<commit_message>
chore: make setup was run
</commit_message>
<xml_diff>
--- a/project/excel/dcatlinkml.xlsx
+++ b/project/excel/dcatlinkml.xlsx
@@ -7,9 +7,44 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="catalog" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="catalogCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="dcat_Dataset" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="dcat_Distribution" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="dcat_Catalog" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="dct_LicenseDocument" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="dcat_DataService" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="dcat_CatalogRecord" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="dct_Location" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="dct_PeriodOfTime" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="foaf_agent" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="DatasetinSeries" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="dcat_DatasetSeries" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="dcat_Resource" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="rdfs_Literal" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="vcard_Kind" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="skos_Concept" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="adms_Identifier" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="foaf_Document" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="dcat_Relationship" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="xsd_decimal" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="xsd_duration" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="dct_Frequency" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="dct_Standard" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="rdfs_Resource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="dct_LinguisticSystem" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="dct_ProvenanceStatement" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="prov_Attribution" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="prov_Activity" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="dct_MediaTypeOrExtent" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="xsd_nonNegativInteger" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="dct_MediaType" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="dct_RightsStatement" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="odrl_hasPolicy" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="spdx_Checksum" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="lcon_Geometry" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="xsd_date" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="xsd_dateTime" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="xsd_gYear" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="xsd_gYearMonth" sheetId="38" state="visible" r:id="rId38"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,17 +461,182 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>dct_description</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>dct_title</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>dct_contactPoint</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dct_keyword</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dct_theme</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>adms_identifier</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>adms_versionNotes</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dcat_landingPage</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dcat_qualifiedRelation</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>dcat_spatialResolutionInMeters</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dcat_temporalResolution</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dcat_version</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dct_accessRights</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dct_accuralPeriodicity</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>dct_conformsTo</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>dct_identifier</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>dct_isReferencedBy</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>dct_issued</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>dct_language</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>dct_modified</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>dct_provenance</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>dct_relation</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>dct_type</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>foaf_page</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>owl_versionInfo</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>prov_qualifiedAttribution</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>prov_wasGeneratedBy</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>dcat_themeTaxonomy</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>dct_spatial</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>dct_temporal</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>dct_publisher</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>dcat_distribution</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>dcat_hasVersion</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>dcat_isVersionOf</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>dct_source</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>adms_sample</t>
         </is>
       </c>
     </row>
@@ -445,13 +645,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,57 +662,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_email</t>
+          <t>dct_description</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>dct_title</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>dct_accuralPeriodicity</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>dcat_prev</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>dcat_next</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>dcat_inSeries</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,11 +713,1065 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>dct_description</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dct_title</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dcat_contactPoint</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dct_accuralPeriodicity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dct_issued</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dct_modified</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dct_spatial</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dct_temporal</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dct_publisher</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>dcat_seriesMember</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dcat_first</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dcat_last</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dcat_accessURL</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dcatap_availability</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dct_description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dct_format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>adms_status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dcat_byteSize</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dcat_compressFormat</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dcat_downloadURL</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dcat_mediaType</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>dcat_packageFormat</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dcat_spatialResolutionInMeters</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dcat_temporalResolution</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dct_conformsTo</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dct_issued</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>dct_language</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>dct_modified</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>dct_rights</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>dct_title</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>foaf_page</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>odrl_hasPolicy</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>spdx_checksum</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>dct_license</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>dcat_accessesService</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dct_description</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dct_title</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dcat_themeTaxonomy</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dct_issued</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dct_language</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dct_modified</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>foaf_homepage</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dct_rights</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dct_publisher</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>dct_license</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dcat_service</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dct_spatial</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dcat_dataset</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dcat_catalog</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>dct_hasPart</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>dct_isPart</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>dct_temporal</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>dcat_record</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>dct_creator</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dct_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dcat_endpointURL</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dct_title</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dcat_endpointDescription</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dct_accessRights</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dct_description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dct_format</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dcat_servesDataset</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dct_license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dct_modified</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>adms_status</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dct_conformsTo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dct_issued</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dct_description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>dct_language</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dct_title</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>foaf_primaryTopic</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>dct_source</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dcat_bbox</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dcat_centroid</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>lcon_geometry</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dcat_endDate</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dcat_startDate</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>time_hasBeginning</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>time_hasEnd</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>foaf_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dct_type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>